<commit_message>
1. LocationName: display on SideMenu, Login Screen. 2. For Inactive User 'Access Denied' message on login screen. 3. Set up - - change LiveSites to DB -
</commit_message>
<xml_diff>
--- a/Documents/FromCustomer/24Mar2017/01. Country Specifc Search Weblinks.xlsx
+++ b/Documents/FromCustomer/24Mar2017/01. Country Specifc Search Weblinks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Country Specific Search'!$A$1:$B$1</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -595,7 +595,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>